<commit_message>
aanvulling beton vuistregels (2)
</commit_message>
<xml_diff>
--- a/book/calculation_examples/concrete/Images/global dimensioning beam concrete.xlsx
+++ b/book/calculation_examples/concrete/Images/global dimensioning beam concrete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roel\SDE-local-clone-github\Structural_Design_Essentials\book\calculation_examples\concrete\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13C5AE3-BAD8-4C02-97E4-4CDED092DDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B849AA-BD49-43D6-AF6D-6F0A83B59D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>b/3</t>
   </si>
@@ -147,12 +147,50 @@
       <t xml:space="preserve"> L / 15</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">  z</t>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">   d   h</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +240,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -229,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -248,20 +294,23 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -282,6 +331,346 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>512099</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>85044</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>149469</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="354" name="Group 353">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E4AAA51-9EB0-0817-A8CF-91AB5C770FAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="10875299" y="11872598"/>
+          <a:ext cx="246970" cy="1035975"/>
+          <a:chOff x="11792630" y="11872598"/>
+          <a:chExt cx="246970" cy="1035975"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="346" name="Straight Connector 345">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00E474E8-ECC4-7407-9D41-9D2A8C594389}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11796714" y="11872598"/>
+            <a:ext cx="0" cy="1035975"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="348" name="Straight Arrow Connector 347">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BE13A56-7732-5425-BDFC-6B145A6DC364}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="11792630" y="11876000"/>
+            <a:ext cx="244928" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:headEnd type="none" w="sm" len="sm"/>
+            <a:tailEnd type="triangle" w="sm" len="sm"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="349" name="Straight Arrow Connector 348">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77856F2B-303C-75E4-F406-74320553C88E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="11792630" y="11938819"/>
+            <a:ext cx="244928" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:headEnd type="none" w="sm" len="sm"/>
+            <a:tailEnd type="triangle" w="sm" len="sm"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="350" name="Straight Arrow Connector 349">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B630135C-A283-9D60-2665-24622FFA8221}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="11792630" y="12000225"/>
+            <a:ext cx="244928" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:headEnd type="none" w="sm" len="sm"/>
+            <a:tailEnd type="triangle" w="sm" len="sm"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="351" name="Straight Arrow Connector 350">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E47190E4-A309-AB48-56BE-46D956CB3EBF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="11792630" y="12063045"/>
+            <a:ext cx="117700" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:headEnd type="none" w="sm" len="sm"/>
+            <a:tailEnd type="triangle" w="sm" len="sm"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="353" name="Freeform: Shape 352">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41E6E510-C971-CD48-57B1-E771F0D242FA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="11796346" y="11875477"/>
+            <a:ext cx="243254" cy="252046"/>
+          </a:xfrm>
+          <a:custGeom>
+            <a:avLst/>
+            <a:gdLst>
+              <a:gd name="csX0" fmla="*/ 243254 w 243254"/>
+              <a:gd name="csY0" fmla="*/ 0 h 252046"/>
+              <a:gd name="csX1" fmla="*/ 243254 w 243254"/>
+              <a:gd name="csY1" fmla="*/ 123092 h 252046"/>
+              <a:gd name="csX2" fmla="*/ 0 w 243254"/>
+              <a:gd name="csY2" fmla="*/ 252046 h 252046"/>
+              <a:gd name="csX3" fmla="*/ 0 w 243254"/>
+              <a:gd name="csY3" fmla="*/ 252046 h 252046"/>
+              <a:gd name="csX4" fmla="*/ 0 w 243254"/>
+              <a:gd name="csY4" fmla="*/ 252046 h 252046"/>
+            </a:gdLst>
+            <a:ahLst/>
+            <a:cxnLst>
+              <a:cxn ang="0">
+                <a:pos x="csX0" y="csY0"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="csX1" y="csY1"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="csX2" y="csY2"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="csX3" y="csY3"/>
+              </a:cxn>
+              <a:cxn ang="0">
+                <a:pos x="csX4" y="csY4"/>
+              </a:cxn>
+            </a:cxnLst>
+            <a:rect l="l" t="t" r="r" b="b"/>
+            <a:pathLst>
+              <a:path w="243254" h="252046">
+                <a:moveTo>
+                  <a:pt x="243254" y="0"/>
+                </a:moveTo>
+                <a:lnTo>
+                  <a:pt x="243254" y="123092"/>
+                </a:lnTo>
+                <a:lnTo>
+                  <a:pt x="0" y="252046"/>
+                </a:lnTo>
+                <a:lnTo>
+                  <a:pt x="0" y="252046"/>
+                </a:lnTo>
+                <a:lnTo>
+                  <a:pt x="0" y="252046"/>
+                </a:lnTo>
+              </a:path>
+            </a:pathLst>
+          </a:custGeom>
+          <a:noFill/>
+          <a:ln w="6350"/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="nl-NL" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -2668,8 +3057,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6031573" y="7713573"/>
-          <a:ext cx="120268" cy="88992"/>
+          <a:off x="6044825" y="7725551"/>
+          <a:ext cx="123581" cy="89502"/>
           <a:chOff x="6671553" y="7428695"/>
           <a:chExt cx="117950" cy="80709"/>
         </a:xfrm>
@@ -2823,8 +3212,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3900638" y="7708859"/>
-          <a:ext cx="113016" cy="88992"/>
+          <a:off x="3900638" y="7720837"/>
+          <a:ext cx="116329" cy="89502"/>
           <a:chOff x="6671553" y="7428695"/>
           <a:chExt cx="117950" cy="80709"/>
         </a:xfrm>
@@ -2978,8 +3367,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1784054" y="7709158"/>
-          <a:ext cx="115632" cy="88992"/>
+          <a:off x="1777428" y="7721136"/>
+          <a:ext cx="112319" cy="89502"/>
           <a:chOff x="6671553" y="7428695"/>
           <a:chExt cx="117950" cy="80709"/>
         </a:xfrm>
@@ -3133,8 +3522,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6035145" y="4545941"/>
-          <a:ext cx="120268" cy="88992"/>
+          <a:off x="6048397" y="4551803"/>
+          <a:ext cx="123581" cy="89501"/>
           <a:chOff x="6671553" y="7428695"/>
           <a:chExt cx="117950" cy="80709"/>
         </a:xfrm>
@@ -3288,8 +3677,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3904210" y="4541227"/>
-          <a:ext cx="113016" cy="88992"/>
+          <a:off x="3904210" y="4547089"/>
+          <a:ext cx="116329" cy="89501"/>
           <a:chOff x="6671553" y="7428695"/>
           <a:chExt cx="117950" cy="80709"/>
         </a:xfrm>
@@ -3443,8 +3832,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1787626" y="4541526"/>
-          <a:ext cx="115632" cy="88992"/>
+          <a:off x="1781000" y="4547388"/>
+          <a:ext cx="112319" cy="89501"/>
           <a:chOff x="6671553" y="7428695"/>
           <a:chExt cx="117950" cy="80709"/>
         </a:xfrm>
@@ -3598,8 +3987,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6038717" y="1384262"/>
-          <a:ext cx="120268" cy="88991"/>
+          <a:off x="6051969" y="1384007"/>
+          <a:ext cx="123581" cy="89501"/>
           <a:chOff x="6671553" y="7428695"/>
           <a:chExt cx="117950" cy="80709"/>
         </a:xfrm>
@@ -3753,8 +4142,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3907782" y="1379548"/>
-          <a:ext cx="113016" cy="88991"/>
+          <a:off x="3907782" y="1379293"/>
+          <a:ext cx="116329" cy="89501"/>
           <a:chOff x="6671553" y="7428695"/>
           <a:chExt cx="117950" cy="80709"/>
         </a:xfrm>
@@ -3908,8 +4297,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1791198" y="1379847"/>
-          <a:ext cx="115632" cy="88991"/>
+          <a:off x="1784572" y="1379592"/>
+          <a:ext cx="112319" cy="89501"/>
           <a:chOff x="6671553" y="7428695"/>
           <a:chExt cx="117950" cy="80709"/>
         </a:xfrm>
@@ -4063,8 +4452,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5016712" y="1415816"/>
-          <a:ext cx="1061900" cy="1612752"/>
+          <a:off x="5023338" y="1415561"/>
+          <a:ext cx="1068526" cy="1616320"/>
           <a:chOff x="9737481" y="2006111"/>
           <a:chExt cx="1071457" cy="1554774"/>
         </a:xfrm>
@@ -4651,8 +5040,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1862185" y="7835379"/>
-          <a:ext cx="1004139" cy="115989"/>
+          <a:off x="1852246" y="7847867"/>
+          <a:ext cx="1007452" cy="116498"/>
           <a:chOff x="1845102" y="7537205"/>
           <a:chExt cx="1009834" cy="107706"/>
         </a:xfrm>
@@ -4768,8 +5157,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="16200000">
-          <a:off x="978902" y="6871202"/>
-          <a:ext cx="1505881" cy="166685"/>
+          <a:off x="971002" y="6881906"/>
+          <a:ext cx="1508429" cy="166685"/>
           <a:chOff x="1845102" y="7537205"/>
           <a:chExt cx="1009834" cy="107706"/>
         </a:xfrm>
@@ -4885,8 +5274,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm flipH="1">
-          <a:off x="2865355" y="7715346"/>
-          <a:ext cx="79611" cy="66941"/>
+          <a:off x="2858729" y="7727324"/>
+          <a:ext cx="82924" cy="67451"/>
           <a:chOff x="6671553" y="7428695"/>
           <a:chExt cx="117950" cy="80709"/>
         </a:xfrm>
@@ -5091,8 +5480,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm flipH="1">
-          <a:off x="4982696" y="1382465"/>
-          <a:ext cx="79610" cy="66940"/>
+          <a:off x="4989322" y="1382210"/>
+          <a:ext cx="82923" cy="67450"/>
           <a:chOff x="6671553" y="7428695"/>
           <a:chExt cx="117950" cy="80709"/>
         </a:xfrm>
@@ -6693,8 +7082,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm flipH="1">
-          <a:off x="1825057" y="6136685"/>
-          <a:ext cx="79611" cy="66941"/>
+          <a:off x="1818431" y="6145604"/>
+          <a:ext cx="76298" cy="67452"/>
           <a:chOff x="6671553" y="7428695"/>
           <a:chExt cx="117950" cy="80709"/>
         </a:xfrm>
@@ -6899,7 +7288,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9902765" y="7115544"/>
+          <a:off x="9899452" y="7127012"/>
           <a:ext cx="415095" cy="384817"/>
           <a:chOff x="9439275" y="5432246"/>
           <a:chExt cx="415095" cy="384611"/>
@@ -7176,8 +7565,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9411646" y="7114244"/>
-          <a:ext cx="433299" cy="340811"/>
+          <a:off x="9411646" y="7125712"/>
+          <a:ext cx="429986" cy="340811"/>
           <a:chOff x="9410700" y="4685550"/>
           <a:chExt cx="429986" cy="338207"/>
         </a:xfrm>
@@ -7413,8 +7802,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11423898" y="4612591"/>
-          <a:ext cx="416970" cy="379610"/>
+          <a:off x="11413959" y="4618962"/>
+          <a:ext cx="413657" cy="380629"/>
           <a:chOff x="9439275" y="5432246"/>
           <a:chExt cx="415095" cy="384611"/>
         </a:xfrm>
@@ -7690,8 +8079,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13414271" y="4612591"/>
-          <a:ext cx="420029" cy="379610"/>
+          <a:off x="13394393" y="4618962"/>
+          <a:ext cx="416716" cy="380629"/>
           <a:chOff x="9439275" y="5432246"/>
           <a:chExt cx="415095" cy="384611"/>
         </a:xfrm>
@@ -8018,8 +8407,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11414170" y="5231636"/>
-          <a:ext cx="416970" cy="379258"/>
+          <a:off x="11404231" y="5239537"/>
+          <a:ext cx="413657" cy="379258"/>
           <a:chOff x="9439275" y="5432246"/>
           <a:chExt cx="415095" cy="384611"/>
         </a:xfrm>
@@ -8295,8 +8684,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13404543" y="5170665"/>
-          <a:ext cx="420029" cy="379434"/>
+          <a:off x="13384665" y="5178055"/>
+          <a:ext cx="416716" cy="379945"/>
           <a:chOff x="9439275" y="5432246"/>
           <a:chExt cx="415095" cy="384611"/>
         </a:xfrm>
@@ -8953,8 +9342,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9411646" y="4609346"/>
-          <a:ext cx="433299" cy="338208"/>
+          <a:off x="9411646" y="4615717"/>
+          <a:ext cx="429986" cy="338718"/>
           <a:chOff x="9410700" y="4685550"/>
           <a:chExt cx="429986" cy="338207"/>
         </a:xfrm>
@@ -9190,8 +9579,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9417089" y="5175640"/>
-          <a:ext cx="433299" cy="338207"/>
+          <a:off x="9417089" y="5183030"/>
+          <a:ext cx="429986" cy="338718"/>
           <a:chOff x="9410700" y="4685550"/>
           <a:chExt cx="429986" cy="338207"/>
         </a:xfrm>
@@ -9764,8 +10153,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="16200000">
-          <a:off x="10008362" y="1605960"/>
-          <a:ext cx="1063797" cy="325887"/>
+          <a:off x="10000717" y="1606724"/>
+          <a:ext cx="1065836" cy="325887"/>
           <a:chOff x="9413447" y="2690132"/>
           <a:chExt cx="1064052" cy="325887"/>
         </a:xfrm>
@@ -11209,8 +11598,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="16200000">
-          <a:off x="13562742" y="1727686"/>
-          <a:ext cx="1163725" cy="179621"/>
+          <a:off x="13535219" y="1728450"/>
+          <a:ext cx="1165764" cy="179621"/>
           <a:chOff x="9299804" y="2690133"/>
           <a:chExt cx="1177696" cy="179621"/>
         </a:xfrm>
@@ -12249,8 +12638,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="16200000">
-          <a:off x="10059648" y="1733549"/>
-          <a:ext cx="1163725" cy="179615"/>
+          <a:off x="10052003" y="1734313"/>
+          <a:ext cx="1165764" cy="179615"/>
           <a:chOff x="9299804" y="2690139"/>
           <a:chExt cx="1177696" cy="179615"/>
         </a:xfrm>
@@ -12603,8 +12992,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11423898" y="8356330"/>
-          <a:ext cx="416970" cy="396175"/>
+          <a:off x="11413959" y="8370346"/>
+          <a:ext cx="413657" cy="401145"/>
           <a:chOff x="9439275" y="5432246"/>
           <a:chExt cx="415095" cy="384611"/>
         </a:xfrm>
@@ -12931,8 +13320,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11414170" y="8991941"/>
-          <a:ext cx="416970" cy="412388"/>
+          <a:off x="11404231" y="9011437"/>
+          <a:ext cx="413657" cy="417358"/>
           <a:chOff x="9439275" y="5432246"/>
           <a:chExt cx="415095" cy="384611"/>
         </a:xfrm>
@@ -13208,8 +13597,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13404543" y="8947535"/>
-          <a:ext cx="420029" cy="404282"/>
+          <a:off x="13384665" y="8967031"/>
+          <a:ext cx="416716" cy="409252"/>
           <a:chOff x="9439275" y="5432246"/>
           <a:chExt cx="415095" cy="384611"/>
         </a:xfrm>
@@ -13485,8 +13874,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9411646" y="8353085"/>
-          <a:ext cx="433299" cy="354774"/>
+          <a:off x="9411646" y="8367101"/>
+          <a:ext cx="429986" cy="359234"/>
           <a:chOff x="9410700" y="4685550"/>
           <a:chExt cx="429986" cy="338207"/>
         </a:xfrm>
@@ -13722,8 +14111,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9417089" y="8935944"/>
-          <a:ext cx="433299" cy="363056"/>
+          <a:off x="9417089" y="8954930"/>
+          <a:ext cx="429986" cy="368025"/>
           <a:chOff x="9410700" y="4685550"/>
           <a:chExt cx="429986" cy="338207"/>
         </a:xfrm>
@@ -14012,8 +14401,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11417482" y="9668128"/>
-          <a:ext cx="416970" cy="412387"/>
+          <a:off x="11407543" y="9693103"/>
+          <a:ext cx="413657" cy="417357"/>
           <a:chOff x="9439275" y="5432246"/>
           <a:chExt cx="415095" cy="384611"/>
         </a:xfrm>
@@ -14289,8 +14678,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13407855" y="9668128"/>
-          <a:ext cx="420029" cy="404281"/>
+          <a:off x="13387977" y="9693103"/>
+          <a:ext cx="416716" cy="409251"/>
           <a:chOff x="9439275" y="5432246"/>
           <a:chExt cx="415095" cy="384611"/>
         </a:xfrm>
@@ -14947,8 +15336,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9420401" y="9643279"/>
-          <a:ext cx="433299" cy="363054"/>
+          <a:off x="9420401" y="9668254"/>
+          <a:ext cx="429986" cy="368024"/>
           <a:chOff x="9410700" y="4685550"/>
           <a:chExt cx="429986" cy="338207"/>
         </a:xfrm>
@@ -15184,8 +15573,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="15332726" y="9643279"/>
-          <a:ext cx="420029" cy="404281"/>
+          <a:off x="15299596" y="9668254"/>
+          <a:ext cx="420029" cy="409251"/>
           <a:chOff x="9439275" y="5432246"/>
           <a:chExt cx="415095" cy="384611"/>
         </a:xfrm>
@@ -15543,6 +15932,2167 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Rectangle 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BF734B0-D8DD-448F-96B6-3B35E9D25D2E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9515475" y="1310309"/>
+          <a:ext cx="727213" cy="1004680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>308882</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>195945</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>195945</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Connector 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6D3F3DE-831B-4299-9B4B-38AE84D5E35B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9452882" y="2606184"/>
+          <a:ext cx="875531" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>385082</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>385082</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>83005</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Straight Connector 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3323CFC4-B2DF-43BD-B73A-5BC4AE721CB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9529082" y="2515015"/>
+          <a:ext cx="0" cy="177012"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>493934</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>493934</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>83005</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Connector 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81FEF195-59EC-4A85-BEA0-182EDAAF2E7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10250847" y="2515015"/>
+          <a:ext cx="0" cy="177012"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>336096</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>159205</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>422933</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Straight Connector 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60F3EF87-FBB6-41BD-B7AA-085ECCF49818}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9480096" y="2569444"/>
+          <a:ext cx="86837" cy="66793"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>450391</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>159205</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>537228</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="Straight Connector 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF10F4FA-E62E-4964-B42E-99FD72D6F8FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10207304" y="2569444"/>
+          <a:ext cx="86837" cy="66793"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>7491</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>2896</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>333378</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>81063</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="50" name="Group 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58720178-BA80-43FF-A271-778541780168}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm rot="16200000">
+          <a:off x="9981667" y="12179474"/>
+          <a:ext cx="1103936" cy="325887"/>
+          <a:chOff x="9413447" y="2690132"/>
+          <a:chExt cx="1064052" cy="325887"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="56" name="Straight Connector 55">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BE8D0D1-A7AD-24C5-38DF-DBDAFD86F196}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000" flipV="1">
+            <a:off x="9945473" y="2249277"/>
+            <a:ext cx="0" cy="1064052"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="81" name="Straight Connector 80">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15C57DCF-BCEE-5BE2-FDC0-B32D9D1FEDC2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9476480" y="2690140"/>
+            <a:ext cx="0" cy="179615"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="82" name="Straight Connector 81">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F86261C-9C27-FAD9-3939-D83DDBE758E0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="10236990" y="2853076"/>
+            <a:ext cx="325887" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="83" name="Straight Connector 82">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C4D7B97-4AC7-1930-0A1C-C8BE0F1B9CE1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="9427495" y="2744562"/>
+            <a:ext cx="86837" cy="69396"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="84" name="Straight Connector 83">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47412897-6CB0-733E-E7E1-E010170D2B8C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="10356391" y="2744562"/>
+            <a:ext cx="86837" cy="69396"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>429986</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>435429</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="85" name="Flowchart: Alternate Process 84">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F22BFD0E-FFED-4DBF-8B84-AF780E13EDB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9573986" y="1364738"/>
+          <a:ext cx="618356" cy="898544"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartAlternateProcess">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>473528</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>135516</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>519247</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>181235</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="86" name="Oval 85">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DB2CFB0-B82A-454F-9787-3800DE5A8723}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9617528" y="1369625"/>
+          <a:ext cx="45719" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>23948</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>135516</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>69667</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>181235</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="152" name="Oval 151">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BD373F7-9066-431B-8743-D8236B0D3EE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9780861" y="1369625"/>
+          <a:ext cx="45719" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>180158</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>135516</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>225877</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>181235</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="158" name="Oval 157">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2663D38-1063-4A67-A9B5-C43D0CBEEDF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9937071" y="1369625"/>
+          <a:ext cx="45719" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>340178</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>135516</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>385897</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>181235</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="160" name="Oval 159">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AC4A099-74C7-49C3-9C39-5B94B52E4E6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10097091" y="1369625"/>
+          <a:ext cx="45719" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>469718</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>181236</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>515437</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>36455</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="161" name="Oval 160">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7925E4DC-6963-4166-8947-E41699A80FE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9613718" y="2210475"/>
+          <a:ext cx="45719" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>20138</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>181236</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>65857</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>36455</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="162" name="Oval 161">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4709F7DB-C01D-4272-B7F5-BF2DD4F4EE67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9777051" y="2210475"/>
+          <a:ext cx="45719" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>176348</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>181236</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>222067</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>36455</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="174" name="Oval 173">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24BCFFD6-5675-4A79-A82E-A3B6DBD08625}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9933261" y="2210475"/>
+          <a:ext cx="45719" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>336368</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>181236</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>382087</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>36455</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="175" name="Oval 174">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCF7801F-2138-40C7-AB9F-B40353BABF2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10093281" y="2210475"/>
+          <a:ext cx="45719" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>430739</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>17993</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>466739</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>53993</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="226" name="Oval 225">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F00B3723-BB7D-4847-88F3-C085D5C78248}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9574739" y="1649667"/>
+          <a:ext cx="36000" cy="36000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>392639</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>17993</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>428639</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>53993</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="227" name="Oval 226">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C6903DF-F4AA-47DC-AF73-58F40189AAD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10149552" y="1649667"/>
+          <a:ext cx="36000" cy="36000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>433666</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>102987</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>469666</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>138987</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="228" name="Oval 227">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{278CB836-86E4-4607-B02E-497DA2F461BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9577666" y="1933444"/>
+          <a:ext cx="36000" cy="36000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>395566</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>102987</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>431566</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>138987</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="229" name="Oval 228">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F172290-0DEE-44E4-A7FF-61D8E5EFF798}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10152479" y="1933444"/>
+          <a:ext cx="36000" cy="36000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>181877</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>7385</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>361492</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>185480</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="296" name="Group 295">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97F639F5-6A98-495A-8459-1B638E2C7DBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm rot="16200000">
+          <a:off x="10032953" y="12307063"/>
+          <a:ext cx="1203864" cy="179615"/>
+          <a:chOff x="9299804" y="2690139"/>
+          <a:chExt cx="1177696" cy="179615"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="297" name="Straight Connector 296">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80F1ECE9-B2BC-2A8E-F6E0-B1B6A2C5BCD5}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000" flipV="1">
+            <a:off x="9888652" y="2192455"/>
+            <a:ext cx="0" cy="1177696"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="298" name="Straight Connector 297">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0F3AFF5-2EE7-6239-6374-A5FA4AF82F9C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9387570" y="2690139"/>
+            <a:ext cx="0" cy="179615"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="299" name="Straight Connector 298">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A78FAC3C-324F-2A18-8FD9-A464CF45DB13}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="9338584" y="2744562"/>
+            <a:ext cx="86837" cy="69396"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="300" name="Straight Connector 299">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{552673BF-9062-9D99-2FC8-085AB418499B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="10356391" y="2744562"/>
+            <a:ext cx="86837" cy="69396"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>521677</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>13282</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>13282</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="301" name="Straight Connector 300">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B08057F2-61DC-4750-AA3C-435B0F834042}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10275277" y="12826605"/>
+          <a:ext cx="1154723" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>403698</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>79443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>44586</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>79443</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="302" name="Straight Connector 301">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{353A5E0A-344D-4C75-924B-EDA4AB115DB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10160611" y="1313552"/>
+          <a:ext cx="253801" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>503922</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>169876</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>169876</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="303" name="Straight Connector 302">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08C77CA6-0791-83E1-13AD-4A6F8DAE255B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10257522" y="11957430"/>
+          <a:ext cx="890538" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>192989</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>102577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>371499</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>83924</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="320" name="Group 319">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB23793E-CD94-0B23-621F-466744B9F85C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm rot="16200000">
+          <a:off x="10751486" y="12304434"/>
+          <a:ext cx="1007116" cy="178510"/>
+          <a:chOff x="9413446" y="2690140"/>
+          <a:chExt cx="913694" cy="179615"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="321" name="Straight Connector 320">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31624938-89E1-3E9F-6F34-C3CED0C8EAD6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000" flipV="1">
+            <a:off x="9870293" y="2324457"/>
+            <a:ext cx="0" cy="913694"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="322" name="Straight Connector 321">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1132B89-4B94-724D-D02A-514CBD5BB293}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9476480" y="2690140"/>
+            <a:ext cx="0" cy="179615"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="323" name="Straight Connector 322">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{705D4716-A352-B1A3-B9FE-6CADCE8B82AE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="10190155" y="2761727"/>
+            <a:ext cx="143173" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="324" name="Straight Connector 323">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{701ED45F-9D1E-985B-CFC9-1CFA45606BF6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="9427495" y="2744562"/>
+            <a:ext cx="86837" cy="69396"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="325" name="Straight Connector 324">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CF47BAA-F497-3618-A01B-1E6FCD3147ED}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="10218197" y="2744571"/>
+            <a:ext cx="86837" cy="69396"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>135984</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>156210</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>14064</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="342" name="Arrow: Right 341">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EA34434-58A2-DE24-302D-B7DD14C4DA6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10873740" y="11923538"/>
+          <a:ext cx="255270" cy="77372"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>156210</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="343" name="Arrow: Right 342">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C9FDA8F-6D51-30DD-1938-4D586D4E5C8B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10873740" y="12900660"/>
+          <a:ext cx="255270" cy="80010"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -15814,10 +18364,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A5:AB51"/>
+  <dimension ref="A5:AB66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N49" sqref="N49"/>
+    <sheetView tabSelected="1" topLeftCell="P57" zoomScale="325" zoomScaleNormal="325" workbookViewId="0">
+      <selection activeCell="U64" sqref="U64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -15832,22 +18382,22 @@
       <c r="C5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10" t="s">
+      <c r="E5" s="13"/>
+      <c r="F5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10" t="s">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10" t="s">
+      <c r="I5" s="13"/>
+      <c r="J5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="10"/>
+      <c r="K5" s="13"/>
       <c r="L5" s="6" t="s">
         <v>0</v>
       </c>
@@ -15861,12 +18411,12 @@
       </c>
     </row>
     <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -15879,24 +18429,24 @@
       </c>
     </row>
     <row r="19" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
     </row>
     <row r="27" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="2"/>
       <c r="V28" s="8"/>
     </row>
@@ -15915,13 +18465,13 @@
       </c>
     </row>
     <row r="36" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B36" s="2"/>
     </row>
     <row r="37" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
+      <c r="A37" s="14"/>
     </row>
     <row r="43" spans="1:25" ht="17.25" x14ac:dyDescent="0.3">
       <c r="V43" s="1" t="s">
@@ -15929,38 +18479,38 @@
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="P44" s="14" t="s">
+      <c r="P44" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="P45" s="14"/>
+      <c r="P45" s="11"/>
     </row>
     <row r="46" spans="1:25" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="P46" s="14"/>
+      <c r="P46" s="11"/>
       <c r="Y46" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="P47" s="14" t="s">
+      <c r="P47" s="11" t="s">
         <v>11</v>
       </c>
       <c r="V47" s="8"/>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="P48" s="14"/>
+      <c r="P48" s="11"/>
       <c r="S48" s="7"/>
       <c r="V48" s="7"/>
     </row>
     <row r="49" spans="16:28" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="P49" s="14"/>
+      <c r="P49" s="11"/>
       <c r="AB49" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="50" spans="16:28" x14ac:dyDescent="0.25">
-      <c r="P50" s="14" t="s">
+      <c r="P50" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -15968,13 +18518,36 @@
       <c r="S51" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="V51" s="13" t="s">
+      <c r="V51" s="10" t="s">
         <v>9</v>
       </c>
       <c r="Y51" s="12" t="s">
         <v>8</v>
       </c>
       <c r="Z51" s="12"/>
+    </row>
+    <row r="61" spans="16:28" ht="18" x14ac:dyDescent="0.35">
+      <c r="T61" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="62" spans="16:28" x14ac:dyDescent="0.25">
+      <c r="S62" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="T62" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="18:20" ht="18" x14ac:dyDescent="0.35">
+      <c r="T65" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R66" s="9" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>